<commit_message>
fix: preprocessing the datasets
</commit_message>
<xml_diff>
--- a/Review Destinasi Wisata Trenggalek/excel/Review_Kolam Renang Sumber Agung.xlsx
+++ b/Review Destinasi Wisata Trenggalek/excel/Review_Kolam Renang Sumber Agung.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Haris\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Haris\OneDrive\Documents\TB Datamine (Datasets)\Review Destinasi Wisata Trenggalek\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7EB1BC8-6498-4150-97E9-98D62CFD038E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F6A554-3D09-4F1E-82A1-3BCA4C866250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>author_title</t>
-  </si>
-  <si>
     <t>review_text</t>
   </si>
   <si>
@@ -38,78 +35,6 @@
   </si>
   <si>
     <t>Kolam Renang Sumber Agung</t>
-  </si>
-  <si>
-    <t>Almira Islamadina</t>
-  </si>
-  <si>
-    <t>Syauqi Mushoffa</t>
-  </si>
-  <si>
-    <t>nunuk mahanani</t>
-  </si>
-  <si>
-    <t>Emha Husnan Wahid</t>
-  </si>
-  <si>
-    <t>Jesicca Aulia</t>
-  </si>
-  <si>
-    <t>Sindia Nurlika</t>
-  </si>
-  <si>
-    <t>Nindy Qory</t>
-  </si>
-  <si>
-    <t>tri santoso</t>
-  </si>
-  <si>
-    <t>Ana Miandani</t>
-  </si>
-  <si>
-    <t>Luthfi Phesek</t>
-  </si>
-  <si>
-    <t>-Paradoxz</t>
-  </si>
-  <si>
-    <t>Reni Rahmawati</t>
-  </si>
-  <si>
-    <t>lina zumrotul</t>
-  </si>
-  <si>
-    <t>Ibnu Ghisyam</t>
-  </si>
-  <si>
-    <t>Pendi Kuyy</t>
-  </si>
-  <si>
-    <t>Aditya EkaW</t>
-  </si>
-  <si>
-    <t>EKA mas duha romatilah</t>
-  </si>
-  <si>
-    <t>Nico Dejavu</t>
-  </si>
-  <si>
-    <t>Wahyu Oktaviani</t>
-  </si>
-  <si>
-    <t>07 Atitar Aliwa Kahfi</t>
-  </si>
-  <si>
-    <t>Irwan Ganescha</t>
-  </si>
-  <si>
-    <t>Davinza Garenk</t>
-  </si>
-  <si>
-    <t>Antin Mayang</t>
-  </si>
-  <si>
-    <t>xeriy bhowo</t>
   </si>
   <si>
     <t>kolam renang nya sepii
@@ -153,27 +78,12 @@
     <t>04/08/2025 09:47:17</t>
   </si>
   <si>
-    <t>11/23/2024 08:42:02</t>
-  </si>
-  <si>
-    <t>11/26/2023 02:46:32</t>
-  </si>
-  <si>
-    <t>05/29/2023 21:58:39</t>
-  </si>
-  <si>
     <t>02/25/2023 02:02:06</t>
   </si>
   <si>
     <t>02/05/2023 01:21:07</t>
   </si>
   <si>
-    <t>11/01/2022 06:49:15</t>
-  </si>
-  <si>
-    <t>03/01/2022 02:22:11</t>
-  </si>
-  <si>
     <t>10/17/2021 07:42:15</t>
   </si>
   <si>
@@ -183,40 +93,19 @@
     <t>01/06/2021 13:02:19</t>
   </si>
   <si>
-    <t>05/21/2020 12:53:11</t>
-  </si>
-  <si>
     <t>12/29/2019 06:42:38</t>
   </si>
   <si>
     <t>10/08/2019 01:47:44</t>
   </si>
   <si>
-    <t>07/02/2019 14:26:27</t>
-  </si>
-  <si>
-    <t>04/23/2019 13:15:36</t>
-  </si>
-  <si>
-    <t>04/09/2019 04:10:31</t>
-  </si>
-  <si>
     <t>02/07/2019 11:01:52</t>
   </si>
   <si>
     <t>01/23/2019 06:53:05</t>
   </si>
   <si>
-    <t>08/12/2018 10:26:52</t>
-  </si>
-  <si>
     <t>04/23/2018 12:16:14</t>
-  </si>
-  <si>
-    <t>04/01/2018 02:49:05</t>
-  </si>
-  <si>
-    <t>02/11/2018 22:45:08</t>
   </si>
   <si>
     <t>02/07/2018 19:10:09</t>
@@ -278,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -289,10 +178,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,20 +485,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ25"/>
+  <dimension ref="A1:AI13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13" style="3" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" customWidth="1"/>
-    <col min="6" max="36" width="8.88671875" style="5"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13" style="3" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.3">
@@ -620,14 +506,11 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -658,374 +541,170 @@
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="3">
+      <c r="C2" s="3">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
-        <v>42</v>
+      <c r="D2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="3">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>43</v>
+        <v>6</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="3">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>44</v>
+      <c r="D4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="3">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>45</v>
+      <c r="D5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>46</v>
+        <v>9</v>
+      </c>
+      <c r="C6" s="3">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="3">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>47</v>
+      <c r="D7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="3">
-        <v>4</v>
-      </c>
-      <c r="E8" t="s">
-        <v>48</v>
+        <v>11</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="3">
-        <v>5</v>
-      </c>
-      <c r="E9" t="s">
-        <v>49</v>
+        <v>12</v>
+      </c>
+      <c r="C9" s="3">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="3">
         <v>5</v>
       </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="3">
-        <v>5</v>
-      </c>
-      <c r="E10" t="s">
-        <v>50</v>
+      <c r="D10" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="3">
+        <v>14</v>
+      </c>
+      <c r="C11" s="3">
         <v>3</v>
       </c>
-      <c r="E11" t="s">
-        <v>51</v>
+      <c r="D11" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="3">
         <v>5</v>
       </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="3">
-        <v>5</v>
-      </c>
-      <c r="E12" t="s">
-        <v>52</v>
+      <c r="D12" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="3">
-        <v>5</v>
-      </c>
-      <c r="E13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="3">
+        <v>16</v>
+      </c>
+      <c r="C13" s="3">
         <v>2</v>
       </c>
-      <c r="E14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="3">
-        <v>3</v>
-      </c>
-      <c r="E15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="3">
-        <v>4</v>
-      </c>
-      <c r="E16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="3">
-        <v>5</v>
-      </c>
-      <c r="E17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="3">
-        <v>3</v>
-      </c>
-      <c r="E18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="3">
-        <v>5</v>
-      </c>
-      <c r="E19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="3">
-        <v>3</v>
-      </c>
-      <c r="E20" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="3">
-        <v>4</v>
-      </c>
-      <c r="E21" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="3">
-        <v>5</v>
-      </c>
-      <c r="E22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="3">
-        <v>1</v>
-      </c>
-      <c r="E23" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="D13" t="s">
         <v>28</v>
-      </c>
-      <c r="D24" s="3">
-        <v>1</v>
-      </c>
-      <c r="E24" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="3">
-        <v>2</v>
-      </c>
-      <c r="E25" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>